<commit_message>
Pre-processing german credit data
</commit_message>
<xml_diff>
--- a/references/observational_definitions_overview.xlsx
+++ b/references/observational_definitions_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elisa\Documents\DTU\Fairness-oriented-interpretability-of-predictive-algorithms\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A210F9-2FCE-4025-8997-76C72ABC2D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C85A00-A7F0-46C0-9E8A-575C0EFDF569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{F64A2A74-1509-4EB9-819E-3E87240B377E}"/>
   </bookViews>
@@ -636,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F26BCFF-2D15-4EB7-8EA2-0978BA503A57}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="119" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>